<commit_message>
Documentation Complete. Submitted To Moodle.
Only the code needs to be completed
</commit_message>
<xml_diff>
--- a/PWI_Tests.xlsx
+++ b/PWI_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Project Files\N-Body\Parallel-N-Body\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9575498-CC13-40C6-A7A6-07F49447A24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F48B4D-4214-444D-8F2A-366AC198C0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01329190-AE8B-4428-BE9B-4FAB065FB5D9}"/>
   </bookViews>
@@ -773,7 +773,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>